<commit_message>
Reports: Examples of reports with successful or failed actions
</commit_message>
<xml_diff>
--- a/TestImportExcelSheet.xlsx
+++ b/TestImportExcelSheet.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="14385"/>
+    <workbookView xWindow="192" yWindow="24" windowWidth="21006" windowHeight="9876"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
-  <si>
-    <t xml:space="preserve">Action </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+  <si>
+    <t>Action</t>
   </si>
   <si>
     <t>Parameter1</t>
@@ -36,43 +36,55 @@
     <t>Parameter5</t>
   </si>
   <si>
+    <t xml:space="preserve">Delay </t>
+  </si>
+  <si>
+    <t>SelectBrand</t>
+  </si>
+  <si>
+    <t>PEUGEOT</t>
+  </si>
+  <si>
+    <t>ModelSelect</t>
+  </si>
+  <si>
+    <t>AUTO</t>
+  </si>
+  <si>
+    <t>LoginUFT</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>SelectButton</t>
+  </si>
+  <si>
+    <t>LaunchApplication</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>Engine management ECU</t>
+  </si>
+  <si>
+    <t>CMM_MD1CS003</t>
+  </si>
+  <si>
+    <t>SelectECU</t>
+  </si>
+  <si>
+    <t>SelectMenu</t>
+  </si>
+  <si>
+    <t>IDENTIFICATION</t>
+  </si>
+  <si>
     <t>LaunchDiagBox</t>
   </si>
   <si>
-    <t>SelectBrand</t>
-  </si>
-  <si>
-    <t>PEUGEOT</t>
-  </si>
-  <si>
-    <t>ModelSelect</t>
-  </si>
-  <si>
-    <t>AUTO</t>
-  </si>
-  <si>
-    <t>Delay</t>
-  </si>
-  <si>
-    <t>SelectButton</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>LaunchApplication</t>
-  </si>
-  <si>
     <t>Fault finding</t>
-  </si>
-  <si>
-    <t>SelectECU</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>SubFamily</t>
   </si>
 </sst>
 </file>
@@ -404,20 +416,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.15625" customWidth="1"/>
+    <col min="2" max="2" width="25.26171875" customWidth="1"/>
+    <col min="3" max="3" width="21.15625" customWidth="1"/>
+    <col min="4" max="4" width="15.578125" customWidth="1"/>
+    <col min="5" max="5" width="14.41796875" customWidth="1"/>
+    <col min="6" max="6" width="18.734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -442,7 +454,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -455,53 +467,82 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>10000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>20000</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -515,7 +556,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -527,7 +568,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>